<commit_message>
fix rf board 3d and fix 42 boot 3d
</commit_message>
<xml_diff>
--- a/3d-model/OutStpFan/dummy_boards_bom.xlsx
+++ b/3d-model/OutStpFan/dummy_boards_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduNetdiskDownload\FANwrok\FanOpenProj\Out_FAN\dummy\3d-model\OutStpFan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduNetdiskDownload\FANwrok\FanOpenProj\dummy_backup\dummy\3d-model\OutStpFan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2231EA-46ED-49D0-AE0E-76FED2EFE328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17224CD-A78D-402D-B5EF-84BAA119BAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REF" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="281">
   <si>
     <t>Comment</t>
   </si>
@@ -427,9 +427,6 @@
   </si>
   <si>
     <t>LQFP-64_N</t>
-  </si>
-  <si>
-    <t>SY8089 2A</t>
   </si>
   <si>
     <t>U3</t>
@@ -966,6 +963,34 @@
   </si>
   <si>
     <t>Joint6_Dummy v164 v3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>颜色</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>亮银色</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>灰色</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>工艺</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>阳极黑化细磨砂喷漆</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>LP2992 3V3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SY8089 2A</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1126,7 +1151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1184,6 +1209,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1461,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2406,17 +2438,17 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="B56" s="7">
+        <v>1</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B56" s="7">
-        <v>1</v>
-      </c>
-      <c r="C56" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>135</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>96</v>
@@ -2424,16 +2456,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="7">
+        <v>1</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B57" s="7">
-        <v>1</v>
-      </c>
-      <c r="C57" s="7" t="s">
+      <c r="D57" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>96</v>
@@ -2450,7 +2482,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2466,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -2483,16 +2515,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>142</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>143</v>
       </c>
       <c r="E2" s="7">
         <v>2</v>
@@ -2503,16 +2535,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="E3" s="7">
         <v>6</v>
@@ -2523,10 +2555,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>65</v>
@@ -2546,13 +2578,13 @@
         <v>84</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
@@ -2563,13 +2595,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>154</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>99</v>
@@ -2586,13 +2618,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
@@ -2606,10 +2638,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>11</v>
@@ -2626,10 +2658,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>99</v>
@@ -2646,10 +2678,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>99</v>
@@ -2666,7 +2698,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>19</v>
@@ -2683,13 +2715,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>161</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>99</v>
@@ -2706,7 +2738,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>30</v>
@@ -2726,10 +2758,10 @@
         <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>99</v>
@@ -2746,10 +2778,10 @@
         <v>34</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>11</v>
@@ -2763,16 +2795,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
@@ -2786,10 +2818,10 @@
         <v>108</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>11</v>
@@ -2806,7 +2838,7 @@
         <v>38</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>25</v>
@@ -2823,13 +2855,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>99</v>
@@ -2846,10 +2878,10 @@
         <v>119</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>121</v>
@@ -2863,16 +2895,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="E21" s="7">
         <v>1</v>
@@ -2886,10 +2918,10 @@
         <v>58</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>60</v>
@@ -2906,10 +2938,10 @@
         <v>61</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>63</v>
@@ -2922,17 +2954,17 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="7">
         <v>1</v>
@@ -2946,10 +2978,10 @@
         <v>64</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>66</v>
@@ -2963,13 +2995,13 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>99</v>
@@ -2986,7 +3018,7 @@
         <v>81</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>88</v>
@@ -3006,10 +3038,10 @@
         <v>87</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>89</v>
@@ -3023,16 +3055,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="E29" s="7">
         <v>1</v>
@@ -3043,16 +3075,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="E30" s="7">
         <v>2</v>
@@ -3063,16 +3095,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="E31" s="7">
         <v>2</v>
@@ -3083,16 +3115,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="E32" s="7">
         <v>1</v>
@@ -3103,13 +3135,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="8" t="s">
         <v>199</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>200</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>94</v>
@@ -3153,7 +3185,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -3173,13 +3205,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>96</v>
@@ -3187,19 +3219,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>96</v>
@@ -3213,10 +3245,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>11</v>
@@ -3233,10 +3265,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>11</v>
@@ -3247,19 +3279,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="7">
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>96</v>
@@ -3267,19 +3299,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>71</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>96</v>
@@ -3287,13 +3319,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>65</v>
@@ -3313,13 +3345,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>96</v>
@@ -3333,10 +3365,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>89</v>
@@ -3347,16 +3379,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" s="7">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>99</v>
@@ -3373,10 +3405,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>11</v>
@@ -3393,10 +3425,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>99</v>
@@ -3413,10 +3445,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>99</v>
@@ -3433,7 +3465,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>19</v>
@@ -3447,16 +3479,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>161</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>99</v>
@@ -3473,7 +3505,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>30</v>
@@ -3493,10 +3525,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>99</v>
@@ -3513,10 +3545,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>11</v>
@@ -3527,19 +3559,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" s="7">
         <v>1</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>8</v>
@@ -3553,10 +3585,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>11</v>
@@ -3573,7 +3605,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>25</v>
@@ -3587,16 +3619,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="7">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="B23" s="7">
-        <v>1</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>99</v>
@@ -3613,7 +3645,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>39</v>
@@ -3627,19 +3659,19 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B25" s="7">
-        <v>1</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>8</v>
@@ -3653,10 +3685,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>60</v>
@@ -3673,10 +3705,10 @@
         <v>2</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>63</v>
@@ -3693,10 +3725,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>66</v>
@@ -3707,16 +3739,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B29" s="7">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>99</v>
@@ -3733,7 +3765,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>88</v>
@@ -3747,19 +3779,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B31" s="7">
-        <v>1</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>8</v>
@@ -3767,19 +3799,19 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B32" s="7">
         <v>2</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>8</v>
@@ -3787,19 +3819,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B33" s="7">
         <v>2</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>8</v>
@@ -3807,19 +3839,19 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="7">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B34" s="7">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>8</v>
@@ -3827,16 +3859,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B35" s="7">
         <v>2</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>199</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>200</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>94</v>
@@ -3867,229 +3899,229 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" s="13">
         <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="13">
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B4" s="13">
         <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B5" s="13">
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" s="13">
         <v>3</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7" s="13">
         <v>2</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="13">
         <v>6</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="13">
         <v>3</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B11" s="13">
         <v>16</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B12" s="13">
         <v>4</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B13" s="13">
         <v>4</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="13">
         <v>12</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B15" s="13">
         <v>4</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B17" s="13">
         <v>4</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B18" s="13">
         <v>12</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B20" s="13">
         <v>4</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B21" s="13">
         <v>4</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B23" s="13">
         <v>12</v>
@@ -4103,20 +4135,20 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B26" s="13">
         <v>5</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -4148,18 +4180,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" t="s">
         <v>241</v>
-      </c>
-      <c r="B1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
         <v>243</v>
-      </c>
-      <c r="B2" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4171,10 +4203,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5314D1-190A-4B5A-B43D-748B5312F06B}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4182,156 +4214,217 @@
     <col min="1" max="1" width="43.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="26"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E7" s="26"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="C2" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="C3" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="C6" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>251</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="C8" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E10" s="26"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>252</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>253</v>
-      </c>
       <c r="B11" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C11" s="13">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E11" s="26"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C12" s="14">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C13" s="14">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="E13" s="26"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:E13"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>